<commit_message>
Add temperature sensor(1,2)+widget FAN
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22207" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23320" uniqueCount="177">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -529,6 +529,24 @@
   </si>
   <si>
     <t xml:space="preserve">Sound:&lt;&gt; C°</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Power: &lt;&gt; C°</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sound: &lt;&gt; C°</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GB-DIRECTION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GB-ALIGNMENT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId43</t>
   </si>
 </sst>
 </file>
@@ -1830,7 +1848,9 @@
         <v>17</v>
       </c>
       <c r="G6"/>
-      <c r="H6"/>
+      <c r="H6" t="s">
+        <v>54</v>
+      </c>
       <c r="I6"/>
       <c r="J6"/>
       <c r="K6" s="7" t="s">
@@ -2040,6 +2060,12 @@
       <c r="F3" t="s">
         <v>36</v>
       </c>
+      <c r="G3" t="s">
+        <v>174</v>
+      </c>
+      <c r="H3" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="4">
       <c r="B4" t="s">
@@ -2480,29 +2506,35 @@
         <v>43</v>
       </c>
       <c r="F29" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="30">
       <c r="B30" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="C30" t="s">
         <v>40</v>
       </c>
       <c r="D30" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="E30" t="s">
         <v>43</v>
       </c>
       <c r="F30" t="s">
-        <v>66</v>
+        <v>173</v>
+      </c>
+      <c r="G30" t="s">
+        <v>43</v>
+      </c>
+      <c r="H30" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="31">
       <c r="B31" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C31" t="s">
         <v>40</v>
@@ -2514,15 +2546,15 @@
         <v>43</v>
       </c>
       <c r="F31" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="32">
       <c r="B32" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C32" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D32" t="s">
         <v>42</v>
@@ -2531,12 +2563,12 @@
         <v>43</v>
       </c>
       <c r="F32" t="s">
-        <v>66</v>
+        <v>162</v>
       </c>
     </row>
     <row r="33">
       <c r="B33" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C33" t="s">
         <v>37</v>
@@ -2548,15 +2580,15 @@
         <v>43</v>
       </c>
       <c r="F33" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row r="34">
       <c r="B34" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C34" t="s">
-        <v>37</v>
+        <v>79</v>
       </c>
       <c r="D34" t="s">
         <v>42</v>
@@ -2565,15 +2597,15 @@
         <v>43</v>
       </c>
       <c r="F34" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="35">
       <c r="B35" t="s">
-        <v>165</v>
+        <v>176</v>
       </c>
       <c r="C35" t="s">
-        <v>79</v>
+        <v>40</v>
       </c>
       <c r="D35" t="s">
         <v>42</v>
@@ -2582,7 +2614,7 @@
         <v>43</v>
       </c>
       <c r="F35" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
analog and digital clock
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23320" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24017" uniqueCount="180">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -547,6 +547,15 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">verdanai.ttf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Big_Clock</t>
   </si>
 </sst>
 </file>
@@ -1980,6 +1989,29 @@
       </c>
     </row>
     <row r="10" spans="2:15">
+      <c r="B10" t="s">
+        <v>179</v>
+      </c>
+      <c r="C10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10">
+        <v>100</v>
+      </c>
+      <c r="E10">
+        <v>4</v>
+      </c>
+      <c r="F10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10"/>
+      <c r="H10" t="s">
+        <v>54</v>
+      </c>
+      <c r="I10"/>
+      <c r="J10" t="s">
+        <v>134</v>
+      </c>
       <c r="K10" s="11" t="s">
         <v>28</v>
       </c>
@@ -2617,6 +2649,23 @@
         <v>172</v>
       </c>
     </row>
+    <row r="36">
+      <c r="B36" t="s">
+        <v>178</v>
+      </c>
+      <c r="C36" t="s">
+        <v>179</v>
+      </c>
+      <c r="D36" t="s">
+        <v>46</v>
+      </c>
+      <c r="E36" t="s">
+        <v>43</v>
+      </c>
+      <c r="F36" t="s">
+        <v>49</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>